<commit_message>
0.3.0 (easier to use; more examples in help page)
</commit_message>
<xml_diff>
--- a/data-raw/provdata_demo.xlsx
+++ b/data-raw/provdata_demo.xlsx
@@ -1,26 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614043BA-5F0C-48CF-9023-B62F8E086B69}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC06869-B95C-4EC4-9AD1-7E2FB58D0E05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="807" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="807" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="prov" sheetId="32" r:id="rId1"/>
+    <sheet name="demo" sheetId="33" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="74">
   <si>
     <t>北京市</t>
   </si>
@@ -238,12 +247,23 @@
   </si>
   <si>
     <t>台湾</t>
+  </si>
+  <si>
+    <t>GDPpc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Province</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -280,9 +300,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -565,7 +586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7247E05-CF70-4BC9-96D6-3165E9EC7E1D}">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1064,4 +1085,275 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{404F6121-0202-457E-89C8-98FEAE047575}">
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>53523.76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>49458.44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2">
+        <v>19544.12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2">
+        <v>17097.28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="2">
+        <v>29088</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2">
+        <v>28024.560000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="2">
+        <v>21947.759999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="2">
+        <v>19167.84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2">
+        <v>56337.599999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="2">
+        <v>37448.36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="2">
+        <v>36182.959999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="2">
+        <v>15020.48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="2">
+        <v>29366.080000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="2">
+        <v>15345.12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="2">
+        <v>28332.44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="2">
+        <v>16984.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="2">
+        <v>20339.84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="2">
+        <v>17627.560000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="2">
+        <v>31964.28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="2">
+        <v>14557.28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="2">
+        <v>17814.04</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="2">
+        <v>20665.599999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="2">
+        <v>15435.64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="2">
+        <v>10808.52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="2">
+        <v>12399.88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="2">
+        <v>13315.6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="2">
+        <v>19173.48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="2">
+        <v>11522.88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="2">
+        <v>17027.88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="2">
+        <v>18364</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" s="2">
+        <v>18297.400000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>